<commit_message>
add helper function to isolate search and use last name due to issues with state website
</commit_message>
<xml_diff>
--- a/arizona/az_nonrehab.xlsx
+++ b/arizona/az_nonrehab.xlsx
@@ -641,7 +641,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
     </row>

</xml_diff>